<commit_message>
- [`nexial-project-inspector`]: *NEW* utility batch file to generate project level information and insight. Current version supports macro and data variable inspection. More enhancement forthcoming. - code update for more efficient System variable definition and default value management.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/macros/artifact/script/MacroLibrary.xlsx
+++ b/examples/macros/artifact/script/MacroLibrary.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B5A326-9505-B341-A1C1-BD1440F21089}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C96AE4-B33B-2842-BAC7-F6B9C42F1797}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="15780" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="487">
   <si>
     <t>description</t>
   </si>
@@ -1533,9 +1533,6 @@
 1. combine command names and urls into CSV
 2. transpose so that we have a CSV of name and url columns
 3. convert to JSON array</t>
-  </si>
-  <si>
-    <t>(empty)</t>
   </si>
 </sst>
 </file>
@@ -3743,7 +3740,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3833,9 +3830,7 @@
       <c r="E3" s="6" t="s">
         <v>482</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>487</v>
-      </c>
+      <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>

</xml_diff>